<commit_message>
Added Decision Trees Notes
</commit_message>
<xml_diff>
--- a/4-Classification Models/Decision Trees/References/C4.5 - Data Validation.xlsx
+++ b/4-Classification Models/Decision Trees/References/C4.5 - Data Validation.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MJ\Manikandan Docs\Machine Learning\DTree\C4.5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\Machine-Learning-101\4-Classification Models\Decision Trees\References\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E807C2F0-63F2-4D70-BF15-A1C897546934}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C8D9A1-D6D0-4BBF-84EB-BBACC0D56AF2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7065" xr2:uid="{42F29B5B-8E72-416B-A43B-B3CCC1E9AB67}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{42F29B5B-8E72-416B-A43B-B3CCC1E9AB67}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Temp" sheetId="1" r:id="rId1"/>
+    <sheet name="Humidity" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="18">
   <si>
     <t>Outlook</t>
   </si>
@@ -75,6 +76,15 @@
   </si>
   <si>
     <t>S(PG|Temp &lt;&gt; X(i))</t>
+  </si>
+  <si>
+    <t>G(PG|Humidity &lt;&gt; X(i))</t>
+  </si>
+  <si>
+    <t>S(PG|Humidity &lt;&gt; X(i))</t>
+  </si>
+  <si>
+    <t>GR(PG|Humidity &lt;&gt; X(i))</t>
   </si>
 </sst>
 </file>
@@ -497,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AC3EDA7-8ACF-4D5C-9AFE-A723703FDBAF}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,10 +1050,570 @@
       <c r="J15" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="A2:F15">
-    <sortCondition ref="B1"/>
+  <sortState ref="A2:J15">
+    <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA611511-396F-411E-97C9-23523CA1AA76}">
+  <dimension ref="A1:J15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1">
+        <v>78</v>
+      </c>
+      <c r="C2" s="1">
+        <v>65</v>
+      </c>
+      <c r="D2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <f>-(5/13) * LOG(5/13, 2) - (8/13) * LOG(8/13, 2)</f>
+        <v>0.96123660472287598</v>
+      </c>
+      <c r="H2" s="4">
+        <f>0.94 - (1/14) * F2 - (13/14) * G2</f>
+        <v>4.7423152757329334E-2</v>
+      </c>
+      <c r="I2" s="4">
+        <f xml:space="preserve"> - (1/14) * LOG(1/14, 2) - (13/14) * LOG(13/14, 2)</f>
+        <v>0.37123232664087563</v>
+      </c>
+      <c r="J2" s="4">
+        <f>H2/I2</f>
+        <v>0.12774521331814337</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>70</v>
+      </c>
+      <c r="C3" s="1">
+        <v>68</v>
+      </c>
+      <c r="D3" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <f>-(5/12) * LOG(5/12, 2) - (7/12) * LOG(7/12, 2)</f>
+        <v>0.97986875665115269</v>
+      </c>
+      <c r="H3" s="4">
+        <f>0.94 - (2/14) * F3 - (12/14) * G3</f>
+        <v>0.10011249429901192</v>
+      </c>
+      <c r="I3" s="4">
+        <f xml:space="preserve"> - (2/14) * LOG(2/14, 2) - (12/14) * LOG(12/14, 2)</f>
+        <v>0.59167277858232747</v>
+      </c>
+      <c r="J3" s="4">
+        <f>H3/I3</f>
+        <v>0.16920246785543458</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
+        <v>76</v>
+      </c>
+      <c r="C4" s="2">
+        <v>70</v>
+      </c>
+      <c r="D4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="4">
+        <f>-(5/10) * LOG(5/10, 2) - (5/10) * LOG(5/10, 2)</f>
+        <v>1</v>
+      </c>
+      <c r="H4" s="4">
+        <f>0.94 - (4/14) * F4 - (10/14) * G4</f>
+        <v>0.22571428571428565</v>
+      </c>
+      <c r="I4" s="4">
+        <f xml:space="preserve"> - (4/14) * LOG(4/14, 2) - (10/14) * LOG(10/14, 2)</f>
+        <v>0.863120568566631</v>
+      </c>
+      <c r="J4" s="4">
+        <f>H4/I4</f>
+        <v>0.26150956648979568</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>92</v>
+      </c>
+      <c r="C5" s="1">
+        <v>70</v>
+      </c>
+      <c r="D5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <f>-(5/10) * LOG(5/10, 2) - (5/10) * LOG(5/10, 2)</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="4">
+        <f>0.94 - (4/14) * F5 - (10/14) * G5</f>
+        <v>0.22571428571428565</v>
+      </c>
+      <c r="I5" s="4">
+        <f xml:space="preserve"> - (4/14) * LOG(4/14, 2) - (10/14) * LOG(10/14, 2)</f>
+        <v>0.863120568566631</v>
+      </c>
+      <c r="J5" s="4">
+        <f>H5/I5</f>
+        <v>0.26150956648979568</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2">
+        <v>70</v>
+      </c>
+      <c r="C6" s="2">
+        <v>72</v>
+      </c>
+      <c r="D6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="4">
+        <f xml:space="preserve"> - (1/5) * LOG(1/5, 2) - (4/5) * LOG(4/5, 2)</f>
+        <v>0.72192809488736231</v>
+      </c>
+      <c r="G6" s="4">
+        <f>-(4/9) * LOG(4/9, 2) - (5/9) * LOG(5/9, 2)</f>
+        <v>0.99107605983822222</v>
+      </c>
+      <c r="H6" s="4">
+        <f>0.94 - (5/14) * F6 - (9/14) * G6</f>
+        <v>4.5048213358513278E-2</v>
+      </c>
+      <c r="I6" s="4">
+        <f xml:space="preserve"> - (5/14) * LOG(5/14, 2) - (9/14) * LOG(9/14, 2)</f>
+        <v>0.94028595867063092</v>
+      </c>
+      <c r="J6" s="4">
+        <f>H6/I6</f>
+        <v>4.7909056753545586E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="1">
+        <v>65</v>
+      </c>
+      <c r="C7" s="1">
+        <v>75</v>
+      </c>
+      <c r="D7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="4">
+        <f xml:space="preserve"> - (1/6) * LOG(1/6, 2) - (5/6) * LOG(5/6, 2)</f>
+        <v>0.65002242164835411</v>
+      </c>
+      <c r="G7" s="4">
+        <f>-(4/8) * LOG(4/8, 2) - (4/8) * LOG(4/8, 2)</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="4">
+        <f>0.94 - (6/14) * F7 - (8/14) * G7</f>
+        <v>8.9990390722133995E-2</v>
+      </c>
+      <c r="I7" s="4">
+        <f xml:space="preserve"> - (6/14) * LOG(6/14, 2) - (8/14) * LOG(8/14, 2)</f>
+        <v>0.98522813603425163</v>
+      </c>
+      <c r="J7" s="4">
+        <f>H7/I7</f>
+        <v>9.1339647570728197E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>68</v>
+      </c>
+      <c r="C8" s="1">
+        <v>76</v>
+      </c>
+      <c r="D8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="4">
+        <f xml:space="preserve"> - (1/7) * LOG(1/7, 2) - (6/7) * LOG(6/7, 2)</f>
+        <v>0.59167277858232747</v>
+      </c>
+      <c r="G8" s="4">
+        <f>-(4/7) * LOG(4/7, 2) - (3/7) * LOG(3/7, 2)</f>
+        <v>0.98522813603425163</v>
+      </c>
+      <c r="H8" s="4">
+        <f>0.94 - (7/14) * F8 - (7/14) * G8</f>
+        <v>0.15154954269171039</v>
+      </c>
+      <c r="I8" s="4">
+        <f xml:space="preserve"> - (7/14) * LOG(7/14, 2) - (7/14) * LOG(7/14, 2)</f>
+        <v>1</v>
+      </c>
+      <c r="J8" s="4">
+        <f>H8/I8</f>
+        <v>0.15154954269171039</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>80</v>
+      </c>
+      <c r="C9" s="2">
+        <v>80</v>
+      </c>
+      <c r="D9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="4">
+        <f xml:space="preserve"> - (2/8) * LOG(2/8, 2) - (6/8) * LOG(6/8, 2)</f>
+        <v>0.81127812445913283</v>
+      </c>
+      <c r="G9" s="4">
+        <f>-(3/6) * LOG(3/6, 2) - (3/6) * LOG(3/6, 2)</f>
+        <v>1</v>
+      </c>
+      <c r="H9" s="4">
+        <f>0.94 - (8/14) * F9 - (6/14) * G9</f>
+        <v>4.7841071737638352E-2</v>
+      </c>
+      <c r="I9" s="4">
+        <f xml:space="preserve"> - (8/14) * LOG(8/14, 2) - (6/14) * LOG(6/14, 2)</f>
+        <v>0.98522813603425163</v>
+      </c>
+      <c r="J9" s="4">
+        <f>H9/I9</f>
+        <v>4.8558369364286147E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2">
+        <v>72</v>
+      </c>
+      <c r="C10" s="2">
+        <v>83</v>
+      </c>
+      <c r="D10" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="4">
+        <f xml:space="preserve"> - (2/9) * LOG(2/9, 2) - (7/9) * LOG(7/9, 2)</f>
+        <v>0.76420450650862026</v>
+      </c>
+      <c r="G10" s="4">
+        <f>-(3/5) * LOG(3/5, 2) - (2/5) * LOG(2/5, 2)</f>
+        <v>0.97095059445466858</v>
+      </c>
+      <c r="H10" s="4">
+        <f>0.94 - (9/14) * F10 - (5/14) * G10</f>
+        <v>0.10195760493921957</v>
+      </c>
+      <c r="I10" s="4">
+        <f xml:space="preserve"> - (9/14) * LOG(9/14, 2) - (5/14) * LOG(5/14, 2)</f>
+        <v>0.94028595867063092</v>
+      </c>
+      <c r="J10" s="4">
+        <f>H10/I10</f>
+        <v>0.1084325507565448</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1">
+        <v>83</v>
+      </c>
+      <c r="C11" s="1">
+        <v>83</v>
+      </c>
+      <c r="D11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="4">
+        <f xml:space="preserve"> - (3/10) * LOG(3/10, 2) - (7/10) * LOG(7/10, 2)</f>
+        <v>0.8812908992306927</v>
+      </c>
+      <c r="G11" s="4">
+        <f>-(2/4) * LOG(2/4, 2) - (2/4) * LOG(2/4, 2)</f>
+        <v>1</v>
+      </c>
+      <c r="H11" s="4">
+        <f>0.94 - (10/14) * F11 - (4/14) * G11</f>
+        <v>2.4792214835219428E-2</v>
+      </c>
+      <c r="I11" s="4">
+        <f xml:space="preserve"> - (10/14) * LOG(10/14, 2) - (4/14) * LOG(4/14, 2)</f>
+        <v>0.863120568566631</v>
+      </c>
+      <c r="J11" s="4">
+        <f t="shared" ref="J11:J14" si="0">H11/I11</f>
+        <v>2.8723930048835958E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2">
+        <v>85</v>
+      </c>
+      <c r="C12" s="2">
+        <v>85</v>
+      </c>
+      <c r="D12" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="4">
+        <f xml:space="preserve"> - (4/11) * LOG(4/11, 2) - (7/11) * LOG(7/11, 2)</f>
+        <v>0.94566030460064021</v>
+      </c>
+      <c r="G12" s="4">
+        <f>-(1/3) * LOG(1/3, 2) - (2/3) * LOG(2/3, 2)</f>
+        <v>0.91829583405448956</v>
+      </c>
+      <c r="H12" s="4">
+        <f>0.94 - (11/14) * F12 - (3/14) * G12</f>
+        <v>2.0351051639205808E-4</v>
+      </c>
+      <c r="I12" s="4">
+        <f xml:space="preserve"> - (11/14) * LOG(11/14, 2) - (3/14) * LOG(3/14, 2)</f>
+        <v>0.74959525725947995</v>
+      </c>
+      <c r="J12" s="4">
+        <f t="shared" si="0"/>
+        <v>2.7149386875270859E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="1">
+        <v>86</v>
+      </c>
+      <c r="C13" s="1">
+        <v>86</v>
+      </c>
+      <c r="D13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="4">
+        <f xml:space="preserve"> - (4/12) * LOG(4/12, 2) - (8/12) * LOG(8/12, 2)</f>
+        <v>0.91829583405448956</v>
+      </c>
+      <c r="G13" s="4">
+        <f>-(1/2) * LOG(1/2, 2) - (1/2) * LOG(1/2, 2)</f>
+        <v>1</v>
+      </c>
+      <c r="H13" s="4">
+        <f>0.94 - (12/14) * F13 - (2/14) * G13</f>
+        <v>1.0032142239009001E-2</v>
+      </c>
+      <c r="I13" s="4">
+        <f xml:space="preserve"> - (12/14) * LOG(12/14, 2) - (2/14) * LOG(2/14, 2)</f>
+        <v>0.59167277858232747</v>
+      </c>
+      <c r="J13" s="4">
+        <f t="shared" si="0"/>
+        <v>1.6955558210817862E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2">
+        <v>75</v>
+      </c>
+      <c r="C14" s="2">
+        <v>89</v>
+      </c>
+      <c r="D14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="4">
+        <f xml:space="preserve"> - (5/13) * LOG(5/13, 2) - (8/13) * LOG(8/13, 2)</f>
+        <v>0.96123660472287598</v>
+      </c>
+      <c r="G14" s="4">
+        <v>0</v>
+      </c>
+      <c r="H14" s="4">
+        <f>0.94 - (13/14) * F14 - (1/14) * G14</f>
+        <v>4.7423152757329334E-2</v>
+      </c>
+      <c r="I14" s="4">
+        <f xml:space="preserve"> - (13/14) * LOG(13/14, 2) - (1/14) * LOG(1/14, 2)</f>
+        <v>0.37123232664087563</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" si="0"/>
+        <v>0.12774521331814337</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2">
+        <v>90</v>
+      </c>
+      <c r="C15" s="2">
+        <v>90</v>
+      </c>
+      <c r="D15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+    </row>
+  </sheetData>
+  <sortState ref="A2:J15">
+    <sortCondition ref="C2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>